<commit_message>
Added the possibility to exclude some patients from the analysis.
</commit_message>
<xml_diff>
--- a/scripts/tests/output/supervised_event_aggregation_results.xlsx
+++ b/scripts/tests/output/supervised_event_aggregation_results.xlsx
@@ -8,16 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\Desktop\workspace\Brugada-Event-Prediction\scripts\tests\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82486BBB-6457-4406-9CA6-EB40C7166761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8EB505-A62F-449F-9E7E-4DB5745F4842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lead_Predictions" sheetId="1" r:id="rId1"/>
     <sheet name="XML_Predictions" sheetId="2" r:id="rId2"/>
     <sheet name="Patient_Predictions" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -851,7 +864,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -874,20 +887,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -898,6 +970,42 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0A6588C0-D03E-4574-8271-BDC893B90E2E}" name="Tabella1" displayName="Tabella1" ref="A1:E157" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:E157" xr:uid="{0A6588C0-D03E-4574-8271-BDC893B90E2E}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="[0, 0, 0]"/>
+        <filter val="[0, 0, 1]"/>
+        <filter val="[0, 0, 2]"/>
+        <filter val="[0, 0]"/>
+        <filter val="[0, 1, 0]"/>
+        <filter val="[0, 1, 1]"/>
+        <filter val="[0, 2, 0]"/>
+        <filter val="[0, 2, 1]"/>
+        <filter val="[0, 2, 2]"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E154">
+    <sortCondition ref="D1:D157"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A2357BED-9D0B-4154-B119-E9E80686C9BE}" name="patient"/>
+    <tableColumn id="2" xr3:uid="{FED1FA69-A1D6-4EDE-98A4-1E60B83713DD}" name="xml_file"/>
+    <tableColumn id="3" xr3:uid="{38ED53FE-4429-4CD1-A602-EE609054D319}" name="num_leads"/>
+    <tableColumn id="4" xr3:uid="{4EA03FCD-1D5C-48F9-8715-AD52E66156C7}" name="lead_predictions"/>
+    <tableColumn id="5" xr3:uid="{74304DD4-1931-44E6-A165-3A705D13DFD2}" name="xml_prediction"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1187,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G468"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="A292" sqref="A281:XFD292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11973,37 +12081,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -12022,90 +12130,90 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -12122,7 +12230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -12139,7 +12247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -12156,7 +12264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -12173,7 +12281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -12192,22 +12300,22 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -12226,39 +12334,39 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -12275,7 +12383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -12292,7 +12400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -12309,7 +12417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -12326,7 +12434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -12343,7 +12451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -12360,7 +12468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -12377,7 +12485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -12396,10 +12504,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -12411,7 +12519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -12428,7 +12536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -12445,7 +12553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -12462,7 +12570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -12479,7 +12587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -12496,7 +12604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -12513,7 +12621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -12530,7 +12638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -12547,7 +12655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -12564,7 +12672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -12581,7 +12689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -12600,10 +12708,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="C37">
         <v>3</v>
@@ -12617,10 +12725,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="C38">
         <v>3</v>
@@ -12632,7 +12740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -12651,10 +12759,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>132</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -12668,10 +12776,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="B41" t="s">
-        <v>59</v>
+        <v>133</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -12685,10 +12793,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>134</v>
       </c>
       <c r="C42">
         <v>3</v>
@@ -12702,10 +12810,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>144</v>
       </c>
       <c r="C43">
         <v>3</v>
@@ -12717,7 +12825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -12736,22 +12844,22 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>148</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="C45">
         <v>3</v>
       </c>
       <c r="D45" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="E45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -12770,27 +12878,27 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>152</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>154</v>
       </c>
       <c r="C47">
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>152</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>156</v>
       </c>
       <c r="C48">
         <v>3</v>
@@ -12804,27 +12912,27 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>158</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>159</v>
       </c>
       <c r="C49">
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>68</v>
+        <v>158</v>
       </c>
       <c r="B50" t="s">
-        <v>70</v>
+        <v>160</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -12836,7 +12944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -12855,22 +12963,22 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>180</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>185</v>
       </c>
       <c r="C52">
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="E52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>68</v>
       </c>
@@ -12889,22 +12997,22 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>180</v>
       </c>
       <c r="B54" t="s">
-        <v>74</v>
+        <v>186</v>
       </c>
       <c r="C54">
         <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="E54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -12923,10 +13031,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>180</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>187</v>
       </c>
       <c r="C56">
         <v>3</v>
@@ -12938,7 +13046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>75</v>
       </c>
@@ -12955,7 +13063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>75</v>
       </c>
@@ -12972,7 +13080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>75</v>
       </c>
@@ -12989,7 +13097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -13006,7 +13114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -13023,7 +13131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -13040,7 +13148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>84</v>
       </c>
@@ -13057,7 +13165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>84</v>
       </c>
@@ -13074,7 +13182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>84</v>
       </c>
@@ -13091,7 +13199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>84</v>
       </c>
@@ -13108,7 +13216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>84</v>
       </c>
@@ -13125,7 +13233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>84</v>
       </c>
@@ -13142,7 +13250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>91</v>
       </c>
@@ -13159,7 +13267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>91</v>
       </c>
@@ -13176,7 +13284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>94</v>
       </c>
@@ -13193,7 +13301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>96</v>
       </c>
@@ -13210,7 +13318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>96</v>
       </c>
@@ -13227,7 +13335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>96</v>
       </c>
@@ -13244,7 +13352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>96</v>
       </c>
@@ -13261,7 +13369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>96</v>
       </c>
@@ -13278,7 +13386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>96</v>
       </c>
@@ -13295,7 +13403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>103</v>
       </c>
@@ -13314,10 +13422,10 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>103</v>
+        <v>202</v>
       </c>
       <c r="B79" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="C79">
         <v>3</v>
@@ -13329,7 +13437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>106</v>
       </c>
@@ -13346,7 +13454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>106</v>
       </c>
@@ -13363,7 +13471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>109</v>
       </c>
@@ -13380,7 +13488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>111</v>
       </c>
@@ -13397,7 +13505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>111</v>
       </c>
@@ -13414,7 +13522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>114</v>
       </c>
@@ -13431,7 +13539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>114</v>
       </c>
@@ -13448,7 +13556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>117</v>
       </c>
@@ -13465,7 +13573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>119</v>
       </c>
@@ -13482,7 +13590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>121</v>
       </c>
@@ -13499,7 +13607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>123</v>
       </c>
@@ -13516,7 +13624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>123</v>
       </c>
@@ -13533,7 +13641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>123</v>
       </c>
@@ -13550,7 +13658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>127</v>
       </c>
@@ -13567,7 +13675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>129</v>
       </c>
@@ -13584,58 +13692,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B95" t="s">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="C95">
         <v>3</v>
       </c>
       <c r="D95" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>131</v>
+        <v>63</v>
       </c>
       <c r="B96" t="s">
-        <v>133</v>
+        <v>64</v>
       </c>
       <c r="C96">
         <v>3</v>
       </c>
       <c r="D96" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B97" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C97">
         <v>3</v>
       </c>
       <c r="D97" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>131</v>
       </c>
@@ -13652,7 +13760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>136</v>
       </c>
@@ -13669,7 +13777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>138</v>
       </c>
@@ -13686,7 +13794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>138</v>
       </c>
@@ -13703,12 +13811,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>141</v>
+        <v>202</v>
       </c>
       <c r="B102" t="s">
-        <v>142</v>
+        <v>206</v>
       </c>
       <c r="C102">
         <v>3</v>
@@ -13720,24 +13828,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>143</v>
+        <v>195</v>
       </c>
       <c r="B103" t="s">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="C103">
         <v>3</v>
       </c>
       <c r="D103" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="E103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>143</v>
       </c>
@@ -13756,39 +13864,39 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="B105" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="C105">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D105" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="E105">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>148</v>
+        <v>7</v>
       </c>
       <c r="B106" t="s">
-        <v>149</v>
+        <v>12</v>
       </c>
       <c r="C106">
         <v>3</v>
       </c>
       <c r="D106" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="E106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>150</v>
       </c>
@@ -13805,7 +13913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>152</v>
       </c>
@@ -13822,24 +13930,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>152</v>
+        <v>68</v>
       </c>
       <c r="B109" t="s">
-        <v>154</v>
+        <v>69</v>
       </c>
       <c r="C109">
         <v>3</v>
       </c>
       <c r="D109" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="E109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>152</v>
       </c>
@@ -13856,24 +13964,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>152</v>
+        <v>68</v>
       </c>
       <c r="B111" t="s">
-        <v>156</v>
+        <v>72</v>
       </c>
       <c r="C111">
         <v>3</v>
       </c>
       <c r="D111" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="E111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>152</v>
       </c>
@@ -13890,75 +13998,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>158</v>
+        <v>68</v>
       </c>
       <c r="B113" t="s">
-        <v>159</v>
+        <v>74</v>
       </c>
       <c r="C113">
         <v>3</v>
       </c>
       <c r="D113" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="E113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>158</v>
+        <v>7</v>
       </c>
       <c r="B114" t="s">
-        <v>160</v>
+        <v>13</v>
       </c>
       <c r="C114">
         <v>3</v>
       </c>
       <c r="D114" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="E114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>158</v>
+        <v>7</v>
       </c>
       <c r="B115" t="s">
-        <v>161</v>
+        <v>16</v>
       </c>
       <c r="C115">
         <v>3</v>
       </c>
       <c r="D115" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="E115">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>162</v>
+        <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>163</v>
+        <v>23</v>
       </c>
       <c r="C116">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D116" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="E116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>162</v>
       </c>
@@ -13975,7 +14083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>162</v>
       </c>
@@ -13992,7 +14100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>166</v>
       </c>
@@ -14009,7 +14117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>166</v>
       </c>
@@ -14026,7 +14134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>166</v>
       </c>
@@ -14043,7 +14151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>170</v>
       </c>
@@ -14060,7 +14168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>170</v>
       </c>
@@ -14077,7 +14185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>170</v>
       </c>
@@ -14094,7 +14202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>170</v>
       </c>
@@ -14111,7 +14219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>170</v>
       </c>
@@ -14128,7 +14236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>170</v>
       </c>
@@ -14145,7 +14253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>170</v>
       </c>
@@ -14162,7 +14270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>170</v>
       </c>
@@ -14179,7 +14287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>170</v>
       </c>
@@ -14196,7 +14304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>180</v>
       </c>
@@ -14213,7 +14321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>180</v>
       </c>
@@ -14230,7 +14338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>180</v>
       </c>
@@ -14247,7 +14355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>180</v>
       </c>
@@ -14264,63 +14372,63 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>180</v>
+        <v>17</v>
       </c>
       <c r="B135" t="s">
-        <v>185</v>
+        <v>25</v>
       </c>
       <c r="C135">
         <v>3</v>
       </c>
       <c r="D135" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="E135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>180</v>
+        <v>7</v>
       </c>
       <c r="B136" t="s">
-        <v>186</v>
+        <v>14</v>
       </c>
       <c r="C136">
         <v>3</v>
       </c>
       <c r="D136" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>180</v>
+        <v>7</v>
       </c>
       <c r="B137" t="s">
-        <v>187</v>
+        <v>15</v>
       </c>
       <c r="C137">
         <v>3</v>
       </c>
       <c r="D137" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E137">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="B138" t="s">
-        <v>188</v>
+        <v>147</v>
       </c>
       <c r="C138">
         <v>3</v>
@@ -14332,7 +14440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>180</v>
       </c>
@@ -14349,7 +14457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>180</v>
       </c>
@@ -14366,7 +14474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>180</v>
       </c>
@@ -14383,7 +14491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>180</v>
       </c>
@@ -14400,7 +14508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>180</v>
       </c>
@@ -14417,7 +14525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>180</v>
       </c>
@@ -14434,7 +14542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>195</v>
       </c>
@@ -14451,7 +14559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>195</v>
       </c>
@@ -14468,7 +14576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>195</v>
       </c>
@@ -14485,7 +14593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>195</v>
       </c>
@@ -14502,24 +14610,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="B149" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C149">
         <v>3</v>
       </c>
       <c r="D149" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="E149">
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>195</v>
       </c>
@@ -14536,24 +14644,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>202</v>
+        <v>63</v>
       </c>
       <c r="B151" t="s">
-        <v>203</v>
+        <v>66</v>
       </c>
       <c r="C151">
         <v>3</v>
       </c>
       <c r="D151" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E151">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>202</v>
       </c>
@@ -14570,7 +14678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>202</v>
       </c>
@@ -14587,24 +14695,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>202</v>
+        <v>158</v>
       </c>
       <c r="B154" t="s">
-        <v>206</v>
+        <v>161</v>
       </c>
       <c r="C154">
         <v>3</v>
       </c>
       <c r="D154" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="E154">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>202</v>
       </c>
@@ -14621,7 +14729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>208</v>
       </c>
@@ -14638,7 +14746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>208</v>
       </c>
@@ -14657,6 +14765,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -14665,7 +14776,7 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="A24:D24"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>